<commit_message>
jury sheet with translations and page break; closes #881
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/jury/Jury.xlsx
+++ b/owlcms/src/main/resources/templates/jury/Jury.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\jury\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79AD74C4-82BD-444D-9123-CDA48C388145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D6DE27-608F-425E-A658-B5192482857A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2805" windowWidth="21600" windowHeight="11295"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Données" sheetId="1" r:id="rId1"/>
@@ -55,55 +55,16 @@
     <definedName name="TAS">Données!#REF!</definedName>
     <definedName name="tirage">Données!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
-    <t>Signature</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Jury member</t>
-  </si>
-  <si>
-    <t>JURY SHEET</t>
-  </si>
-  <si>
-    <t>A - Number of attempts</t>
-  </si>
-  <si>
-    <t>B - Incomplete Attempts</t>
-  </si>
-  <si>
-    <t>D - Errors Made</t>
-  </si>
-  <si>
-    <t>E - Correct Decisions (C-D)</t>
-  </si>
-  <si>
-    <t>F - Score (E / C)</t>
-  </si>
-  <si>
-    <t>C - Assessed Lifts (A-B)</t>
-  </si>
-  <si>
     <t>${session.name}</t>
   </si>
   <si>
@@ -164,9 +125,6 @@
     <t>${t.get("Results.Clean_and_Jerk")}</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
     <t>&lt;jx:forEach items="${athletes}" var="l" varStatus="lifterLoop"&gt;</t>
   </si>
   <si>
@@ -180,15 +138,48 @@
   </si>
   <si>
     <t>${l.entryTotal}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.JurySheet")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.JuryMember")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.Level")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.Signature")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.Score")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.A")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.B")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.C")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.D")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.E")}</t>
+  </si>
+  <si>
+    <t>${t.get("Jury.F")}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="173" formatCode="0;\(0\)"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="0;\(0\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -525,14 +516,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -541,7 +532,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -552,29 +543,29 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -582,68 +573,52 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -651,10 +626,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -662,7 +633,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -674,35 +645,27 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -722,36 +685,44 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Emphase 1" xfId="1"/>
-    <cellStyle name="Emphase 2" xfId="2"/>
-    <cellStyle name="Emphase 3" xfId="3"/>
-    <cellStyle name="Lien hypertexte 2" xfId="4"/>
+    <cellStyle name="Emphase 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Emphase 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Emphase 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Lien hypertexte 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Titre 1" xfId="7"/>
-    <cellStyle name="Titre 1 1" xfId="8"/>
-    <cellStyle name="Titre 1 1 1" xfId="9"/>
-    <cellStyle name="Titre 1 1 1 1" xfId="10"/>
-    <cellStyle name="Titre 1 1 1 1 1" xfId="11"/>
-    <cellStyle name="Titre de la feuille" xfId="12"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Titre 1" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Titre 1 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Titre 1 1 1" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Titre 1 1 1 1" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Titre 1 1 1 1 1" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Titre de la feuille" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1274,13 +1245,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -1300,87 +1271,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="30"/>
+      <c r="A1" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="43" t="s">
-        <v>12</v>
+      <c r="A2" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="29"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52" t="s">
+      <c r="A3" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="29"/>
+      <c r="J3" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="29"/>
+      <c r="I4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,41 +1359,41 @@
       <c r="B6" s="4"/>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="F6" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="62"/>
+      <c r="F6" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="51"/>
+      <c r="K6" s="53"/>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="28">
-        <v>1</v>
-      </c>
-      <c r="G7" s="28">
+      <c r="G7" s="9">
         <v>2</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="41">
         <v>3</v>
       </c>
-      <c r="I7" s="45">
+      <c r="I7" s="38">
         <v>1</v>
       </c>
       <c r="J7" s="9">
@@ -1434,41 +1405,41 @@
     </row>
     <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>36</v>
+      <c r="A9" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="59"/>
+      <c r="D9" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="46"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -1488,18 +1459,18 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="66"/>
+      <c r="A13" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="47"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="66"/>
+      <c r="G13" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="47"/>
       <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -1514,18 +1485,18 @@
       <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="66"/>
+      <c r="A15" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="47"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="13"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15"/>
@@ -1544,75 +1515,75 @@
     </row>
     <row r="18" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="37" t="s">
-        <v>31</v>
+      <c r="B18" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="33" t="s">
-        <v>9</v>
+      <c r="F18" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
+      <c r="B19" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
+      <c r="B20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
+      <c r="B21" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
@@ -1626,220 +1597,220 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="22"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="22"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="22"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="22"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="22"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="22"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="22"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="22"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
+      <c r="C30" s="5"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
     </row>
     <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="22"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
+      <c r="C31" s="5"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="22"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
+      <c r="C32" s="5"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
     </row>
     <row r="33" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="22"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
+      <c r="C33" s="5"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" spans="3:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="22"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
+      <c r="C34" s="5"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
     </row>
     <row r="35" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="22"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="22"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="22"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="22"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="22"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="22"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="22"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="22"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="22"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="22"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="22"/>
+      <c r="C45" s="5"/>
     </row>
     <row r="46" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="22"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="22"/>
+      <c r="C47" s="5"/>
     </row>
     <row r="48" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="22"/>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="22"/>
+      <c r="C49" s="5"/>
     </row>
     <row r="50" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="22"/>
+      <c r="C50" s="5"/>
     </row>
     <row r="51" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="22"/>
+      <c r="C51" s="5"/>
     </row>
     <row r="52" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="22"/>
+      <c r="C52" s="5"/>
     </row>
     <row r="53" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="22"/>
+      <c r="C53" s="5"/>
     </row>
     <row r="54" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="22"/>
+      <c r="C54" s="5"/>
     </row>
     <row r="55" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="22"/>
+      <c r="C55" s="5"/>
     </row>
     <row r="56" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="22"/>
+      <c r="C56" s="5"/>
     </row>
     <row r="57" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C57" s="22"/>
+      <c r="C57" s="5"/>
     </row>
     <row r="58" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C58" s="22"/>
+      <c r="C58" s="5"/>
     </row>
     <row r="59" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C59" s="22"/>
+      <c r="C59" s="5"/>
     </row>
     <row r="60" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C60" s="22"/>
+      <c r="C60" s="5"/>
     </row>
     <row r="61" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="22"/>
+      <c r="C61" s="5"/>
     </row>
     <row r="62" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="22"/>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C63" s="22"/>
+      <c r="C63" s="5"/>
     </row>
     <row r="64" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C64" s="22"/>
+      <c r="C64" s="5"/>
     </row>
     <row r="65" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="22"/>
+      <c r="C65" s="5"/>
     </row>
     <row r="66" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="22"/>
+      <c r="C66" s="5"/>
     </row>
     <row r="67" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="22"/>
+      <c r="C67" s="5"/>
     </row>
     <row r="68" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="22"/>
+      <c r="C68" s="5"/>
     </row>
     <row r="69" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C69" s="22"/>
+      <c r="C69" s="5"/>
     </row>
     <row r="70" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C70" s="22"/>
+      <c r="C70" s="5"/>
     </row>
     <row r="71" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C71" s="22"/>
+      <c r="C71" s="5"/>
     </row>
     <row r="72" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C72" s="22"/>
+      <c r="C72" s="5"/>
     </row>
     <row r="73" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C73" s="22"/>
+      <c r="C73" s="5"/>
     </row>
     <row r="74" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C74" s="22"/>
+      <c r="C74" s="5"/>
     </row>
     <row r="75" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C75" s="22"/>
+      <c r="C75" s="5"/>
     </row>
     <row r="76" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C76" s="22"/>
+      <c r="C76" s="5"/>
     </row>
     <row r="77" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C77" s="22"/>
+      <c r="C77" s="5"/>
     </row>
     <row r="78" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="22"/>
+      <c r="C78" s="5"/>
     </row>
     <row r="79" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C79" s="22"/>
+      <c r="C79" s="5"/>
     </row>
     <row r="80" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C80" s="22"/>
+      <c r="C80" s="5"/>
     </row>
     <row r="81" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C81" s="22"/>
+      <c r="C81" s="5"/>
     </row>
     <row r="82" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C82" s="22"/>
+      <c r="C82" s="5"/>
     </row>
     <row r="83" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C83" s="22"/>
+      <c r="C83" s="5"/>
     </row>
     <row r="84" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C84" s="22"/>
+      <c r="C84" s="5"/>
     </row>
     <row r="85" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85" s="22"/>
+      <c r="C85" s="5"/>
     </row>
     <row r="86" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C86" s="22"/>
+      <c r="C86" s="5"/>
     </row>
     <row r="87" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C87" s="22"/>
+      <c r="C87" s="5"/>
     </row>
     <row r="88" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C88" s="22"/>
+      <c r="C88" s="5"/>
     </row>
     <row r="89" spans="3:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C89" s="22"/>
+      <c r="C89" s="5"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -1847,26 +1818,26 @@
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14:C14 B17:C22 C13:C21 B12:C12">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+  <conditionalFormatting sqref="B9:B10 B11:C11">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11 B9:B10">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="B12:C12 C13:C21 B14:C14 B17:C22">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1881,17 +1852,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C6">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="G10">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="G10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.74803149606299213" header="0" footer="0"/>
-  <pageSetup scale="75" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="78" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>